<commit_message>
Melhor rede escolhida - 46
</commit_message>
<xml_diff>
--- a/Estudo.xlsx
+++ b/Estudo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\CR\isec-trabalho-cr\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{340F2C28-A5B0-4B1A-88FD-DC7AF5ABD21F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB9616C1-6FD4-4D93-8135-049307761277}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11385" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GREEK a)" sheetId="1" r:id="rId1"/>
@@ -921,7 +921,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
@@ -1535,8 +1535,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DE0E5DA-99CC-4959-BC56-3D33B6AFEA12}">
   <dimension ref="A1:J51"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="G53" sqref="G53"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="I46" sqref="I46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2557,10 +2557,10 @@
       </c>
       <c r="G46" s="1"/>
       <c r="H46" s="3">
-        <v>0.68</v>
+        <v>0.91</v>
       </c>
       <c r="I46" s="3">
-        <v>3.3933999999999999E-2</v>
+        <v>2.0809999999999999E-2</v>
       </c>
       <c r="J46" s="4" t="s">
         <v>29</v>

</xml_diff>

<commit_message>
Começo da alinea c - ler da pasta 3 e simular
</commit_message>
<xml_diff>
--- a/Estudo.xlsx
+++ b/Estudo.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\CR\isec-trabalho-cr\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB9616C1-6FD4-4D93-8135-049307761277}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0538A85D-21EA-4A9D-A225-B9D6B64DC955}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11385" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GREEK a)" sheetId="1" r:id="rId1"/>
     <sheet name="GREEK b)" sheetId="2" r:id="rId2"/>
+    <sheet name="GREEK c)" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="489" uniqueCount="70">
   <si>
     <t>Função de treino</t>
   </si>
@@ -1535,8 +1536,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DE0E5DA-99CC-4959-BC56-3D33B6AFEA12}">
   <dimension ref="A1:J51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="I46" sqref="I46"/>
+    <sheetView topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="I50" sqref="I50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2677,10 +2678,10 @@
       </c>
       <c r="G50" s="1"/>
       <c r="H50" s="3">
-        <v>1</v>
+        <v>0.98</v>
       </c>
       <c r="I50" s="3">
-        <v>3.6817000000000003E-2</v>
+        <v>5.1534000000000003E-2</v>
       </c>
       <c r="J50" s="4" t="s">
         <v>29</v>
@@ -2728,4 +2729,1063 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60710A4B-FBBA-4B41-93EB-8E5D259A11EA}">
+  <dimension ref="A1:J51"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L6" sqref="L6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="28" style="8" customWidth="1"/>
+    <col min="2" max="2" width="18" style="8" customWidth="1"/>
+    <col min="3" max="3" width="14.5" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.625" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15" style="8" customWidth="1"/>
+    <col min="7" max="7" width="5.625" style="8" customWidth="1"/>
+    <col min="8" max="8" width="11" style="8"/>
+    <col min="9" max="9" width="13.875" style="8" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="11" style="8"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:10" ht="45.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="1">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1">
+        <v>10</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" s="1"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:10" ht="56.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="12"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="12"/>
+      <c r="H6" s="12"/>
+      <c r="I6" s="12"/>
+      <c r="J6" s="12"/>
+    </row>
+    <row r="7" spans="1:10" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="6">
+        <v>2</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G7" s="1"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" s="6">
+        <v>2</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G8" s="1"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" s="9">
+        <v>3</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G9" s="1"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" s="9">
+        <v>6</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G10" s="1"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="56.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="12"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="12"/>
+      <c r="I12" s="12"/>
+      <c r="J12" s="12"/>
+    </row>
+    <row r="13" spans="1:10" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B13" s="1">
+        <v>1</v>
+      </c>
+      <c r="C13" s="1">
+        <v>10</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G13" s="1"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B14" s="1">
+        <v>1</v>
+      </c>
+      <c r="C14" s="1">
+        <v>10</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G14" s="1"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B15" s="1">
+        <v>1</v>
+      </c>
+      <c r="C15" s="1">
+        <v>10</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E15" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G15" s="1"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
+      <c r="J15" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B16" s="1">
+        <v>1</v>
+      </c>
+      <c r="C16" s="1">
+        <v>10</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E16" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G16" s="1"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
+      <c r="J16" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B17" s="1">
+        <v>1</v>
+      </c>
+      <c r="C17" s="1">
+        <v>10</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E17" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G17" s="1"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
+      <c r="J17" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B18" s="1">
+        <v>1</v>
+      </c>
+      <c r="C18" s="1">
+        <v>10</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E18" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G18" s="1"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3"/>
+      <c r="J18" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="56.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B21" s="12"/>
+      <c r="C21" s="12"/>
+      <c r="D21" s="12"/>
+      <c r="E21" s="12"/>
+      <c r="F21" s="12"/>
+      <c r="G21" s="12"/>
+      <c r="H21" s="12"/>
+      <c r="I21" s="12"/>
+      <c r="J21" s="12"/>
+    </row>
+    <row r="22" spans="1:10" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B22" s="1">
+        <v>1</v>
+      </c>
+      <c r="C22" s="1">
+        <v>10</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E22" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G22" s="1"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="3"/>
+      <c r="J22" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B23" s="1">
+        <v>1</v>
+      </c>
+      <c r="C23" s="1">
+        <v>10</v>
+      </c>
+      <c r="D23" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="E23" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G23" s="1"/>
+      <c r="H23" s="3"/>
+      <c r="I23" s="3"/>
+      <c r="J23" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B24" s="1">
+        <v>1</v>
+      </c>
+      <c r="C24" s="1">
+        <v>10</v>
+      </c>
+      <c r="D24" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="E24" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G24" s="1"/>
+      <c r="H24" s="3"/>
+      <c r="I24" s="3"/>
+      <c r="J24" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B25" s="1">
+        <v>1</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D25" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E25" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G25" s="1"/>
+      <c r="H25" s="3"/>
+      <c r="I25" s="3"/>
+      <c r="J25" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B26" s="1">
+        <v>1</v>
+      </c>
+      <c r="C26" s="1">
+        <v>10</v>
+      </c>
+      <c r="D26" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E26" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G26" s="1"/>
+      <c r="H26" s="3"/>
+      <c r="I26" s="3"/>
+      <c r="J26" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B27" s="1">
+        <v>1</v>
+      </c>
+      <c r="C27" s="1">
+        <v>10</v>
+      </c>
+      <c r="D27" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="E27" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G27" s="1"/>
+      <c r="H27" s="3"/>
+      <c r="I27" s="3"/>
+      <c r="J27" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" ht="56.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B29" s="12"/>
+      <c r="C29" s="12"/>
+      <c r="D29" s="12"/>
+      <c r="E29" s="12"/>
+      <c r="F29" s="12"/>
+      <c r="G29" s="12"/>
+      <c r="H29" s="12"/>
+      <c r="I29" s="12"/>
+      <c r="J29" s="12"/>
+    </row>
+    <row r="30" spans="1:10" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B30" s="1">
+        <v>1</v>
+      </c>
+      <c r="C30" s="1">
+        <v>10</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F30" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G30" s="1"/>
+      <c r="H30" s="3"/>
+      <c r="I30" s="3"/>
+      <c r="J30" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B31" s="1">
+        <v>1</v>
+      </c>
+      <c r="C31" s="1">
+        <v>10</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F31" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="G31" s="1"/>
+      <c r="H31" s="3"/>
+      <c r="I31" s="3"/>
+      <c r="J31" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B32" s="1">
+        <v>1</v>
+      </c>
+      <c r="C32" s="1">
+        <v>10</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F32" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="G32" s="1"/>
+      <c r="H32" s="3"/>
+      <c r="I32" s="3"/>
+      <c r="J32" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B33" s="1">
+        <v>1</v>
+      </c>
+      <c r="C33" s="1">
+        <v>10</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F33" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="G33" s="1"/>
+      <c r="H33" s="3"/>
+      <c r="I33" s="3"/>
+      <c r="J33" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B34" s="1">
+        <v>1</v>
+      </c>
+      <c r="C34" s="1">
+        <v>10</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F34" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="G34" s="1"/>
+      <c r="H34" s="3"/>
+      <c r="I34" s="3"/>
+      <c r="J34" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B35" s="1">
+        <v>1</v>
+      </c>
+      <c r="C35" s="1">
+        <v>10</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F35" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="G35" s="1"/>
+      <c r="H35" s="3"/>
+      <c r="I35" s="3"/>
+      <c r="J35" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" ht="55.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="B37" s="12"/>
+      <c r="C37" s="12"/>
+      <c r="D37" s="12"/>
+      <c r="E37" s="12"/>
+      <c r="F37" s="12"/>
+      <c r="G37" s="12"/>
+      <c r="H37" s="12"/>
+      <c r="I37" s="12"/>
+      <c r="J37" s="12"/>
+    </row>
+    <row r="38" spans="1:10" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B38" s="1">
+        <v>1</v>
+      </c>
+      <c r="C38" s="1">
+        <v>10</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F38" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="G38" s="1"/>
+      <c r="H38" s="3"/>
+      <c r="I38" s="3"/>
+      <c r="J38" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B39" s="1">
+        <v>1</v>
+      </c>
+      <c r="C39" s="1">
+        <v>10</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F39" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="G39" s="1"/>
+      <c r="H39" s="3"/>
+      <c r="I39" s="3"/>
+      <c r="J39" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B40" s="1">
+        <v>1</v>
+      </c>
+      <c r="C40" s="1">
+        <v>10</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F40" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="G40" s="1"/>
+      <c r="H40" s="3"/>
+      <c r="I40" s="3"/>
+      <c r="J40" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" ht="55.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="B42" s="12"/>
+      <c r="C42" s="12"/>
+      <c r="D42" s="12"/>
+      <c r="E42" s="12"/>
+      <c r="F42" s="12"/>
+      <c r="G42" s="12"/>
+      <c r="H42" s="12"/>
+      <c r="I42" s="12"/>
+      <c r="J42" s="12"/>
+    </row>
+    <row r="43" spans="1:10" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="5">
+        <v>1</v>
+      </c>
+      <c r="B43" s="9">
+        <v>6</v>
+      </c>
+      <c r="C43" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E43" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="F43" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="G43" s="1"/>
+      <c r="H43" s="3"/>
+      <c r="I43" s="3"/>
+      <c r="J43" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="5">
+        <v>2</v>
+      </c>
+      <c r="B44" s="9">
+        <v>6</v>
+      </c>
+      <c r="C44" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E44" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="F44" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="G44" s="1"/>
+      <c r="H44" s="3"/>
+      <c r="I44" s="3"/>
+      <c r="J44" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="5">
+        <v>3</v>
+      </c>
+      <c r="B45" s="9">
+        <v>6</v>
+      </c>
+      <c r="C45" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E45" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="F45" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="G45" s="1"/>
+      <c r="H45" s="3"/>
+      <c r="I45" s="3"/>
+      <c r="J45" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="5">
+        <v>4</v>
+      </c>
+      <c r="B46" s="9">
+        <v>6</v>
+      </c>
+      <c r="C46" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E46" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="F46" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="G46" s="1"/>
+      <c r="H46" s="3"/>
+      <c r="I46" s="3"/>
+      <c r="J46" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="5">
+        <v>5</v>
+      </c>
+      <c r="B47" s="9">
+        <v>6</v>
+      </c>
+      <c r="C47" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E47" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="F47" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="G47" s="1"/>
+      <c r="H47" s="3"/>
+      <c r="I47" s="3"/>
+      <c r="J47" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="5">
+        <v>6</v>
+      </c>
+      <c r="B48" s="9">
+        <v>6</v>
+      </c>
+      <c r="C48" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E48" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="F48" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="G48" s="1"/>
+      <c r="H48" s="3"/>
+      <c r="I48" s="3"/>
+      <c r="J48" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="5">
+        <v>7</v>
+      </c>
+      <c r="B49" s="9">
+        <v>6</v>
+      </c>
+      <c r="C49" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E49" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="F49" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="G49" s="1"/>
+      <c r="H49" s="3"/>
+      <c r="I49" s="3"/>
+      <c r="J49" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" ht="48" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="5">
+        <v>8</v>
+      </c>
+      <c r="B50" s="9">
+        <v>6</v>
+      </c>
+      <c r="C50" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E50" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="F50" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="G50" s="1"/>
+      <c r="H50" s="3"/>
+      <c r="I50" s="3"/>
+      <c r="J50" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" ht="48" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="5">
+        <v>9</v>
+      </c>
+      <c r="B51" s="9">
+        <v>6</v>
+      </c>
+      <c r="C51" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E51" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="F51" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="G51" s="1"/>
+      <c r="H51" s="3"/>
+      <c r="I51" s="3"/>
+      <c r="J51" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="A6:J6"/>
+    <mergeCell ref="A12:J12"/>
+    <mergeCell ref="A21:J21"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A37:J37"/>
+    <mergeCell ref="A42:J42"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
treino pasta 3 e testes 1 2 3
</commit_message>
<xml_diff>
--- a/Estudo.xlsx
+++ b/Estudo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\CR\isec-trabalho-cr\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABD455D6-18B8-4071-9A39-97C09D6AE391}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73D2DFE5-E839-4FBF-A258-4C8C2853B49E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2757,7 +2757,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2810,28 +2810,82 @@
       <c r="A5" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="B5" s="8"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
+      <c r="B5" s="8">
+        <v>0.1</v>
+      </c>
+      <c r="C5" s="8">
+        <v>0.4</v>
+      </c>
+      <c r="D5" s="8">
+        <v>0.4</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="B6" s="8"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
+      <c r="B6" s="8">
+        <v>0.24</v>
+      </c>
+      <c r="C6" s="8">
+        <v>0.35</v>
+      </c>
+      <c r="D6" s="8">
+        <v>0.39</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="B7" s="8"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
+      <c r="B7" s="8">
+        <v>0.6</v>
+      </c>
+      <c r="C7" s="8">
+        <v>0.4</v>
+      </c>
+      <c r="D7" s="8">
+        <v>0.92500000000000004</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:D2">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B5:D5">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B6:D6">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B7:D7">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>

<commit_message>
Inspetor angelo, bug estranho no greek_d
</commit_message>
<xml_diff>
--- a/Estudo.xlsx
+++ b/Estudo.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\CR\isec-trabalho-cr\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44306AA5-2D4B-4ABA-8D33-4753DCCDDB7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FD373D2-8E1F-463A-8809-AC87FBCDF249}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GREEK a)" sheetId="1" r:id="rId1"/>
     <sheet name="GREEK b)" sheetId="2" r:id="rId2"/>
     <sheet name="GREEK c)" sheetId="4" r:id="rId3"/>
+    <sheet name="GREEK d)" sheetId="6" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="79">
   <si>
     <t>Função de treino</t>
   </si>
@@ -264,6 +265,9 @@
   </si>
   <si>
     <t>TREINO DE REDE COM TODAS AS PASTAS</t>
+  </si>
+  <si>
+    <t>caracteres</t>
   </si>
 </sst>
 </file>
@@ -2759,8 +2763,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4C038B8-04A9-4F6E-9564-257A27AAB193}">
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D12" sqref="A1:D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2864,13 +2868,13 @@
         <v>75</v>
       </c>
       <c r="B10" s="8">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="C10" s="8">
         <v>1</v>
       </c>
       <c r="D10" s="8">
-        <v>0.5</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -2878,13 +2882,13 @@
         <v>76</v>
       </c>
       <c r="B11" s="8">
-        <v>0.73</v>
+        <v>0.81</v>
       </c>
       <c r="C11" s="8">
-        <v>1</v>
+        <v>0.95</v>
       </c>
       <c r="D11" s="8">
-        <v>0.41</v>
+        <v>0.57999999999999996</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -2892,13 +2896,260 @@
         <v>73</v>
       </c>
       <c r="B12" s="8">
+        <v>0.77500000000000002</v>
+      </c>
+      <c r="C12" s="8">
+        <v>0.99</v>
+      </c>
+      <c r="D12" s="8">
         <v>0.57499999999999996</v>
       </c>
-      <c r="C12" s="8">
-        <v>1</v>
-      </c>
-      <c r="D12" s="8">
-        <v>0.5</v>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="B2:D2">
+    <cfRule type="colorScale" priority="7">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B5:D5">
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B6:D6">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B7:D7">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B10:D10">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B11:D11">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B12:D12">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2F7B45C-2FF1-4A56-89A7-3EE8A73E0C59}">
+  <dimension ref="A1:D21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="35.25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="8">
+        <v>1</v>
+      </c>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="8">
+        <v>2</v>
+      </c>
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="8">
+        <v>3</v>
+      </c>
+      <c r="B4" s="8"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="8">
+        <v>4</v>
+      </c>
+      <c r="B5" s="8"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="8">
+        <v>5</v>
+      </c>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="8">
+        <v>6</v>
+      </c>
+      <c r="B7" s="8"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="8">
+        <v>8</v>
+      </c>
+      <c r="B9" s="8"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="8">
+        <v>9</v>
+      </c>
+      <c r="B10" s="8"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="8">
+        <v>10</v>
+      </c>
+      <c r="B11" s="8"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="8">
+        <v>11</v>
+      </c>
+      <c r="B12" s="8"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="8">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="8">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="8">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="8">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="8">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="8">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="8">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="8">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="8">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
desculpa zé, tava a morrer, só quero dormir
</commit_message>
<xml_diff>
--- a/Estudo.xlsx
+++ b/Estudo.xlsx
@@ -5,12 +5,12 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\CR\isec-trabalho-cr\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\isec-trabalho-cr\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56FF54C5-2E87-4C43-8C7F-687527637B8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7C0457E-8295-4B61-8F4D-C1A439F86FB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3585" yWindow="1500" windowWidth="21600" windowHeight="11385" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GREEK a)" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="146">
   <si>
     <t>Função de treino</t>
   </si>
@@ -430,6 +430,45 @@
   </si>
   <si>
     <t>net52</t>
+  </si>
+  <si>
+    <t>target</t>
+  </si>
+  <si>
+    <t>α</t>
+  </si>
+  <si>
+    <t>β</t>
+  </si>
+  <si>
+    <t>γ</t>
+  </si>
+  <si>
+    <t>ε</t>
+  </si>
+  <si>
+    <t>η</t>
+  </si>
+  <si>
+    <t>θ</t>
+  </si>
+  <si>
+    <t>π</t>
+  </si>
+  <si>
+    <t>ρ</t>
+  </si>
+  <si>
+    <t>ψ</t>
+  </si>
+  <si>
+    <t>ω</t>
+  </si>
+  <si>
+    <t>✓</t>
+  </si>
+  <si>
+    <t>✗</t>
   </si>
 </sst>
 </file>
@@ -726,17 +765,17 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="73">
@@ -1248,18 +1287,18 @@
     </row>
     <row r="4" spans="1:12" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="6" spans="1:12" ht="56.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="19" t="s">
+      <c r="A6" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="20"/>
-      <c r="C6" s="20"/>
-      <c r="D6" s="20"/>
-      <c r="E6" s="20"/>
-      <c r="F6" s="20"/>
-      <c r="G6" s="20"/>
-      <c r="H6" s="20"/>
-      <c r="I6" s="20"/>
-      <c r="J6" s="20"/>
+      <c r="B6" s="22"/>
+      <c r="C6" s="22"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="22"/>
+      <c r="F6" s="22"/>
+      <c r="G6" s="22"/>
+      <c r="H6" s="22"/>
+      <c r="I6" s="22"/>
+      <c r="J6" s="22"/>
     </row>
     <row r="7" spans="1:12" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
@@ -1406,18 +1445,18 @@
       </c>
     </row>
     <row r="12" spans="1:12" ht="56.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="19" t="s">
+      <c r="A12" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="20"/>
-      <c r="C12" s="20"/>
-      <c r="D12" s="20"/>
-      <c r="E12" s="20"/>
-      <c r="F12" s="20"/>
-      <c r="G12" s="20"/>
-      <c r="H12" s="20"/>
-      <c r="I12" s="20"/>
-      <c r="J12" s="20"/>
+      <c r="B12" s="22"/>
+      <c r="C12" s="22"/>
+      <c r="D12" s="22"/>
+      <c r="E12" s="22"/>
+      <c r="F12" s="22"/>
+      <c r="G12" s="22"/>
+      <c r="H12" s="22"/>
+      <c r="I12" s="22"/>
+      <c r="J12" s="22"/>
     </row>
     <row r="13" spans="1:12" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
@@ -1708,18 +1747,18 @@
       </c>
     </row>
     <row r="23" spans="1:12" ht="56.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="19" t="s">
+      <c r="A23" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="B23" s="20"/>
-      <c r="C23" s="20"/>
-      <c r="D23" s="20"/>
-      <c r="E23" s="20"/>
-      <c r="F23" s="20"/>
-      <c r="G23" s="20"/>
-      <c r="H23" s="20"/>
-      <c r="I23" s="20"/>
-      <c r="J23" s="20"/>
+      <c r="B23" s="22"/>
+      <c r="C23" s="22"/>
+      <c r="D23" s="22"/>
+      <c r="E23" s="22"/>
+      <c r="F23" s="22"/>
+      <c r="G23" s="22"/>
+      <c r="H23" s="22"/>
+      <c r="I23" s="22"/>
+      <c r="J23" s="22"/>
     </row>
     <row r="24" spans="1:12" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
@@ -2058,20 +2097,20 @@
     </row>
     <row r="4" spans="1:14" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="6" spans="1:14" ht="56.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="19" t="s">
+      <c r="A6" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="20"/>
-      <c r="C6" s="20"/>
-      <c r="D6" s="20"/>
-      <c r="E6" s="20"/>
-      <c r="F6" s="20"/>
-      <c r="G6" s="20"/>
-      <c r="H6" s="20"/>
-      <c r="I6" s="20"/>
-      <c r="J6" s="20"/>
-      <c r="K6" s="20"/>
-      <c r="L6" s="20"/>
+      <c r="B6" s="22"/>
+      <c r="C6" s="22"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="22"/>
+      <c r="F6" s="22"/>
+      <c r="G6" s="22"/>
+      <c r="H6" s="22"/>
+      <c r="I6" s="22"/>
+      <c r="J6" s="22"/>
+      <c r="K6" s="22"/>
+      <c r="L6" s="22"/>
     </row>
     <row r="7" spans="1:14" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
@@ -2242,20 +2281,20 @@
       </c>
     </row>
     <row r="12" spans="1:14" ht="56.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="19" t="s">
+      <c r="A12" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="20"/>
-      <c r="C12" s="20"/>
-      <c r="D12" s="20"/>
-      <c r="E12" s="20"/>
-      <c r="F12" s="20"/>
-      <c r="G12" s="20"/>
-      <c r="H12" s="20"/>
-      <c r="I12" s="20"/>
-      <c r="J12" s="20"/>
-      <c r="K12" s="20"/>
-      <c r="L12" s="20"/>
+      <c r="B12" s="22"/>
+      <c r="C12" s="22"/>
+      <c r="D12" s="22"/>
+      <c r="E12" s="22"/>
+      <c r="F12" s="22"/>
+      <c r="G12" s="22"/>
+      <c r="H12" s="22"/>
+      <c r="I12" s="22"/>
+      <c r="J12" s="22"/>
+      <c r="K12" s="22"/>
+      <c r="L12" s="22"/>
     </row>
     <row r="13" spans="1:14" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
@@ -2594,20 +2633,20 @@
       </c>
     </row>
     <row r="23" spans="1:14" ht="56.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="19" t="s">
+      <c r="A23" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="B23" s="20"/>
-      <c r="C23" s="20"/>
-      <c r="D23" s="20"/>
-      <c r="E23" s="20"/>
-      <c r="F23" s="20"/>
-      <c r="G23" s="20"/>
-      <c r="H23" s="20"/>
-      <c r="I23" s="20"/>
-      <c r="J23" s="20"/>
-      <c r="K23" s="20"/>
-      <c r="L23" s="20"/>
+      <c r="B23" s="22"/>
+      <c r="C23" s="22"/>
+      <c r="D23" s="22"/>
+      <c r="E23" s="22"/>
+      <c r="F23" s="22"/>
+      <c r="G23" s="22"/>
+      <c r="H23" s="22"/>
+      <c r="I23" s="22"/>
+      <c r="J23" s="22"/>
+      <c r="K23" s="22"/>
+      <c r="L23" s="22"/>
     </row>
     <row r="24" spans="1:14" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
@@ -2862,20 +2901,20 @@
       </c>
     </row>
     <row r="31" spans="1:14" ht="56.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="19" t="s">
+      <c r="A31" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="B31" s="20"/>
-      <c r="C31" s="20"/>
-      <c r="D31" s="20"/>
-      <c r="E31" s="20"/>
-      <c r="F31" s="20"/>
-      <c r="G31" s="20"/>
-      <c r="H31" s="20"/>
-      <c r="I31" s="20"/>
-      <c r="J31" s="20"/>
-      <c r="K31" s="20"/>
-      <c r="L31" s="20"/>
+      <c r="B31" s="22"/>
+      <c r="C31" s="22"/>
+      <c r="D31" s="22"/>
+      <c r="E31" s="22"/>
+      <c r="F31" s="22"/>
+      <c r="G31" s="22"/>
+      <c r="H31" s="22"/>
+      <c r="I31" s="22"/>
+      <c r="J31" s="22"/>
+      <c r="K31" s="22"/>
+      <c r="L31" s="22"/>
     </row>
     <row r="32" spans="1:14" ht="39.950000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="5" t="s">
@@ -3130,20 +3169,20 @@
       </c>
     </row>
     <row r="39" spans="1:14" ht="55.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="19" t="s">
+      <c r="A39" s="21" t="s">
         <v>63</v>
       </c>
-      <c r="B39" s="20"/>
-      <c r="C39" s="20"/>
-      <c r="D39" s="20"/>
-      <c r="E39" s="20"/>
-      <c r="F39" s="20"/>
-      <c r="G39" s="20"/>
-      <c r="H39" s="20"/>
-      <c r="I39" s="20"/>
-      <c r="J39" s="20"/>
-      <c r="K39" s="20"/>
-      <c r="L39" s="20"/>
+      <c r="B39" s="22"/>
+      <c r="C39" s="22"/>
+      <c r="D39" s="22"/>
+      <c r="E39" s="22"/>
+      <c r="F39" s="22"/>
+      <c r="G39" s="22"/>
+      <c r="H39" s="22"/>
+      <c r="I39" s="22"/>
+      <c r="J39" s="22"/>
+      <c r="K39" s="22"/>
+      <c r="L39" s="22"/>
     </row>
     <row r="40" spans="1:14" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="5" t="s">
@@ -3272,20 +3311,20 @@
       </c>
     </row>
     <row r="44" spans="1:14" ht="55.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="19" t="s">
+      <c r="A44" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="B44" s="20"/>
-      <c r="C44" s="20"/>
-      <c r="D44" s="20"/>
-      <c r="E44" s="20"/>
-      <c r="F44" s="20"/>
-      <c r="G44" s="20"/>
-      <c r="H44" s="20"/>
-      <c r="I44" s="20"/>
-      <c r="J44" s="20"/>
-      <c r="K44" s="20"/>
-      <c r="L44" s="20"/>
+      <c r="B44" s="22"/>
+      <c r="C44" s="22"/>
+      <c r="D44" s="22"/>
+      <c r="E44" s="22"/>
+      <c r="F44" s="22"/>
+      <c r="G44" s="22"/>
+      <c r="H44" s="22"/>
+      <c r="I44" s="22"/>
+      <c r="J44" s="22"/>
+      <c r="K44" s="22"/>
+      <c r="L44" s="22"/>
     </row>
     <row r="45" spans="1:14" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="5">
@@ -3642,7 +3681,7 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3674,19 +3713,19 @@
       <c r="A2" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="B2" s="21">
+      <c r="B2" s="19">
         <v>0.85</v>
       </c>
-      <c r="C2" s="21">
+      <c r="C2" s="19">
         <v>0.75</v>
       </c>
-      <c r="D2" s="22">
+      <c r="D2" s="20">
         <v>0.875</v>
       </c>
-      <c r="E2" s="21">
+      <c r="E2" s="19">
         <v>0.95</v>
       </c>
-      <c r="F2" s="21">
+      <c r="F2" s="19">
         <v>0.7</v>
       </c>
     </row>
@@ -3708,19 +3747,19 @@
       <c r="A5" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="B5" s="21">
+      <c r="B5" s="19">
         <v>0.1</v>
       </c>
-      <c r="C5" s="21">
+      <c r="C5" s="19">
         <v>0.5</v>
       </c>
-      <c r="D5" s="21">
+      <c r="D5" s="19">
         <v>0.1</v>
       </c>
-      <c r="E5" s="21">
+      <c r="E5" s="19">
         <v>0.5</v>
       </c>
-      <c r="F5" s="21">
+      <c r="F5" s="19">
         <v>0.3</v>
       </c>
     </row>
@@ -3728,19 +3767,19 @@
       <c r="A6" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="B6" s="21">
+      <c r="B6" s="19">
         <v>0.14000000000000001</v>
       </c>
-      <c r="C6" s="21">
+      <c r="C6" s="19">
         <v>0.53</v>
       </c>
-      <c r="D6" s="21">
+      <c r="D6" s="19">
         <v>0.11</v>
       </c>
-      <c r="E6" s="21">
+      <c r="E6" s="19">
         <v>0.61</v>
       </c>
-      <c r="F6" s="21">
+      <c r="F6" s="19">
         <v>0.28999999999999998</v>
       </c>
     </row>
@@ -3748,19 +3787,19 @@
       <c r="A7" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="B7" s="21">
+      <c r="B7" s="19">
         <v>0.4</v>
       </c>
-      <c r="C7" s="22">
+      <c r="C7" s="20">
         <v>0.92500000000000004</v>
       </c>
-      <c r="D7" s="21">
+      <c r="D7" s="19">
         <v>0.35</v>
       </c>
-      <c r="E7" s="21">
-        <v>1</v>
-      </c>
-      <c r="F7" s="21">
+      <c r="E7" s="19">
+        <v>1</v>
+      </c>
+      <c r="F7" s="19">
         <v>0.7</v>
       </c>
     </row>
@@ -3776,19 +3815,19 @@
       <c r="A10" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="B10" s="21">
-        <v>1</v>
-      </c>
-      <c r="C10" s="21">
-        <v>1</v>
-      </c>
-      <c r="D10" s="21">
-        <v>1</v>
-      </c>
-      <c r="E10" s="21">
-        <v>1</v>
-      </c>
-      <c r="F10" s="21">
+      <c r="B10" s="19">
+        <v>1</v>
+      </c>
+      <c r="C10" s="19">
+        <v>1</v>
+      </c>
+      <c r="D10" s="19">
+        <v>1</v>
+      </c>
+      <c r="E10" s="19">
+        <v>1</v>
+      </c>
+      <c r="F10" s="19">
         <v>1</v>
       </c>
     </row>
@@ -3796,19 +3835,19 @@
       <c r="A11" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="B11" s="21">
+      <c r="B11" s="19">
         <v>0.99</v>
       </c>
-      <c r="C11" s="21">
-        <v>1</v>
-      </c>
-      <c r="D11" s="21">
-        <v>1</v>
-      </c>
-      <c r="E11" s="21">
-        <v>1</v>
-      </c>
-      <c r="F11" s="21">
+      <c r="C11" s="19">
+        <v>1</v>
+      </c>
+      <c r="D11" s="19">
+        <v>1</v>
+      </c>
+      <c r="E11" s="19">
+        <v>1</v>
+      </c>
+      <c r="F11" s="19">
         <v>1</v>
       </c>
     </row>
@@ -3816,19 +3855,19 @@
       <c r="A12" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="B12" s="21">
+      <c r="B12" s="19">
         <v>0.95</v>
       </c>
-      <c r="C12" s="22">
+      <c r="C12" s="20">
         <v>0.77500000000000002</v>
       </c>
-      <c r="D12" s="22">
+      <c r="D12" s="20">
         <v>0.92500000000000004</v>
       </c>
-      <c r="E12" s="21">
+      <c r="E12" s="19">
         <v>0.95</v>
       </c>
-      <c r="F12" s="21">
+      <c r="F12" s="19">
         <v>1</v>
       </c>
     </row>
@@ -4020,162 +4059,231 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2F7B45C-2FF1-4A56-89A7-3EE8A73E0C59}">
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="35.25" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.25" customWidth="1"/>
+    <col min="3" max="3" width="6.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>71</v>
       </c>
       <c r="B1" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="C1" s="8" t="s">
         <v>131</v>
       </c>
-      <c r="C1" s="8"/>
       <c r="D1" s="8"/>
       <c r="E1" s="8"/>
       <c r="F1" s="8"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" s="8"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="8">
         <v>1</v>
       </c>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
+      <c r="B2" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="C2" t="s">
+        <v>145</v>
+      </c>
       <c r="D2" s="8"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E2" s="8"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
         <v>2</v>
       </c>
-      <c r="B3" s="8"/>
+      <c r="B3" s="8" t="s">
+        <v>135</v>
+      </c>
       <c r="C3" s="8"/>
       <c r="D3" s="8"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E3" s="8"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="8">
         <v>3</v>
       </c>
-      <c r="B4" s="8"/>
+      <c r="B4" s="8" t="s">
+        <v>136</v>
+      </c>
       <c r="C4" s="8"/>
       <c r="D4" s="8"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E4" s="8"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="8">
         <v>4</v>
       </c>
-      <c r="B5" s="8"/>
+      <c r="B5" s="8" t="s">
+        <v>137</v>
+      </c>
       <c r="C5" s="8"/>
       <c r="D5" s="8"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E5" s="8"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="8">
         <v>5</v>
       </c>
-      <c r="B6" s="8"/>
+      <c r="B6" s="8" t="s">
+        <v>138</v>
+      </c>
       <c r="C6" s="8"/>
       <c r="D6" s="8"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E6" s="8"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="8">
         <v>6</v>
       </c>
-      <c r="B7" s="8"/>
+      <c r="B7" s="8" t="s">
+        <v>139</v>
+      </c>
       <c r="C7" s="8"/>
       <c r="D7" s="8"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E7" s="8"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="8">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B8" s="8" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="8">
         <v>8</v>
       </c>
-      <c r="B9" s="8"/>
+      <c r="B9" s="8" t="s">
+        <v>141</v>
+      </c>
       <c r="C9" s="8"/>
       <c r="D9" s="8"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E9" s="8"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="8">
         <v>9</v>
       </c>
-      <c r="B10" s="8"/>
+      <c r="B10" s="8" t="s">
+        <v>142</v>
+      </c>
       <c r="C10" s="8"/>
       <c r="D10" s="8"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E10" s="8"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="8">
         <v>10</v>
       </c>
-      <c r="B11" s="8"/>
+      <c r="B11" s="8" t="s">
+        <v>143</v>
+      </c>
       <c r="C11" s="8"/>
       <c r="D11" s="8"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E11" s="8"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="8">
         <v>11</v>
       </c>
-      <c r="B12" s="8"/>
+      <c r="B12" s="8" t="s">
+        <v>134</v>
+      </c>
       <c r="C12" s="8"/>
       <c r="D12" s="8"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E12" s="8"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="8">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B13" s="8" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="8">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B14" s="8" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="8">
         <v>14</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B15" s="8" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="8">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B16" s="8" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="8">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B17" s="8" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="8">
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B18" s="8" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="8">
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B19" s="8" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="8">
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B20" s="8" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="8">
         <v>20</v>
       </c>
+      <c r="B21" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="C21" t="s">
+        <v>144</v>
+      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B2:D2">
+  <conditionalFormatting sqref="D2:E2">
     <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="min"/>
@@ -4187,7 +4295,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B5:D5">
+  <conditionalFormatting sqref="C5:E5">
     <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="min"/>
@@ -4199,7 +4307,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B6:D6">
+  <conditionalFormatting sqref="C6:E6">
     <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>
@@ -4211,7 +4319,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B7:D7">
+  <conditionalFormatting sqref="C7:E7">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
@@ -4223,7 +4331,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B10:D10">
+  <conditionalFormatting sqref="C10:E10">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
@@ -4235,7 +4343,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B11:D11">
+  <conditionalFormatting sqref="C11:E11">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -4247,7 +4355,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B12:D12">
+  <conditionalFormatting sqref="C12:E12">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -4260,5 +4368,6 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>